<commit_message>
Adding in Tracking URLs
</commit_message>
<xml_diff>
--- a/scripts/twitter_text_templates.xlsx
+++ b/scripts/twitter_text_templates.xlsx
@@ -87,15 +87,9 @@
     <t>94 + 23 = 117</t>
   </si>
   <si>
-    <t>People are more than their #disease. We’re looking for participants @KeckMedUSC #ClinicalTrial http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>107 + 23 = 130</t>
   </si>
   <si>
-    <t>Never underestimate the power of people. We’re looking for participants @KeckMedUSC #disease #ClinicalTrial http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>79 + 23 = 102</t>
   </si>
   <si>
@@ -108,15 +102,9 @@
     <t>87 + 23 = 110</t>
   </si>
   <si>
-    <t>#disease is an important topic. We’re looking for solutions @KeckMedUSC. #ClinicalTrial http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>104 + 23 = 127</t>
   </si>
   <si>
-    <t>It starts with volunteers. We’re looking for research participants @KeckMedUSC - #disease #ClinicalTrial http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>114 + 23 = 137</t>
   </si>
   <si>
@@ -147,9 +135,6 @@
     <t>105 + 23 = 128</t>
   </si>
   <si>
-    <t>Join researcher Principal Investigator’s Name @KeckMedUSC in fighting #disease. Share this #ClinicalTrial http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>General, recruiting</t>
   </si>
   <si>
@@ -159,9 +144,6 @@
     <t>92 + 23 = 115</t>
   </si>
   <si>
-    <t>You may be eligible to aid in this #ClinicalTrial on #disease @KeckMedUSC. We’d appreciate your help http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>Your participation in this #disease #ClinicalTrial @KeckMedUSC could benefit many people. Learn more http://bit.ly/1234567</t>
   </si>
   <si>
@@ -171,9 +153,6 @@
     <t>113 + 23 = 136</t>
   </si>
   <si>
-    <t>Ever wanted to participate in a #ClinicalTrial? Here’s your chance to help advance #disease research http://bit.ly/1234567 @KeckMedUSC</t>
-  </si>
-  <si>
     <t>You may be eligible. This #ClinicalTrial on #disease @KeckMedUSC is now accepting participants http://bit.ly/1234567</t>
   </si>
   <si>
@@ -186,9 +165,6 @@
     <t>Are you a cigarette smoker? You may be eligible to participate in this #ClinicalTrial @KeckMedUSC on #disease http://bit.ly/1234567</t>
   </si>
   <si>
-    <t>You’re more than your #disease. And you may be a unique way to fight it. Participate in #ClinicalTrial @KeckMedUSC http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>Know someone who wants to quit #smoking? We need help to find participants for this #ClinicalTrial @KeckMedUSC http://bit.ly/1234567</t>
   </si>
   <si>
@@ -225,12 +201,6 @@
     <t>Join us! Our #ClinicalTrial participants make it possible to fight #disease in new ways @KeckMedUSC http://bit.ly/1234567</t>
   </si>
   <si>
-    <t>Join Principal Investigator’s Name in fighting #disease by participating in this #ClinicalTrial @KeckMedUSC http://bit.ly/1234567</t>
-  </si>
-  <si>
-    <t>Diagnosed with #disease? Leading researcher PI’s Name @KeckMedUSC is looking for #ClinicalTrial participants http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>#ClinicalTrials are crucial to develop better treatments for #disease. View this new study @KeckMedUSC  http://bit.ly/1234567</t>
   </si>
   <si>
@@ -255,21 +225,12 @@
     <t>Pls share! Know someone who might be interested in participating in this #disease research study @KeckMedUSC?  http://bit.ly/1234567</t>
   </si>
   <si>
-    <t>Patients may hold the key to fighting  #disease. We’re looking for participants @KeckMedUSC #ClincialTrial http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>More science, less fear. Learn more about this  #disease #ClinicalTrial @KeckMedUSC http://bit.ly/1234567</t>
   </si>
   <si>
-    <t>Please RT: We’re decoding the mystery of #disease @KeckMedUSC  &amp; are looking for study participants #ClinicalTrial http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>We want to unlock  #disease &amp; are looking for research participants #ClinicalTrial @KeckMedUSC http://bit.ly/123456</t>
   </si>
   <si>
-    <t>#disease e-patients: We’re looking for your help. Researchers @KeckMedUSC are looking for #ClinicalTrial  volunteers http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>Help improve the health of others! Researchers @KeckMedUSC are looking for participants in  #disease #ClinicalTrial http://bit.ly/1234567</t>
   </si>
   <si>
@@ -291,9 +252,6 @@
     <t>This #ClinicalTrial @KeckMedUSC on #disease is looking for participants.  Pls contact the study team to learn more http://bit.ly/1234567</t>
   </si>
   <si>
-    <t>If you’ve been diagnosed with #disease, you could help us fight it. Participate in this #ClinicalTrial @KeckMedUSC  http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>Please help us work toward a cure for #disease by participating in this #ClinicalTrial @KeckMedUSC  http://bit.ly/1234567</t>
   </si>
   <si>
@@ -306,16 +264,58 @@
     <t>#disease #ClinicalTrials give hope to many patients &amp; their families. Participate @KeckMedUSC. Eligibility  http://bit.ly/1234567</t>
   </si>
   <si>
-    <t xml:space="preserve">We cannot  find better #disease treatments without you. If you’re eligible, pls participate @KeckMedUSC http://bit.ly/1234567 </t>
-  </si>
-  <si>
     <t>It starts with you! Please participate in our #ClinicalTrial on  #disease @KeckMedUSC http://bit.ly/1234567</t>
   </si>
   <si>
-    <t>You can make a difference in others’ lives. Please participate in our #ClinicalTrial on  #disease @KeckMedUSC http://bit.ly/1234567</t>
-  </si>
-  <si>
     <t>Message type</t>
+  </si>
+  <si>
+    <t>Patients may hold the key to fighting  #disease. We're looking for participants @KeckMedUSC #ClincialTrial http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>People are more than their #disease. We're looking for participants @KeckMedUSC #ClinicalTrial http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>Never underestimate the power of people. We're looking for participants @KeckMedUSC #disease #ClinicalTrial http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>#disease is an important topic. We're looking for solutions @KeckMedUSC. #ClinicalTrial http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>It starts with volunteers. We're looking for research participants @KeckMedUSC - #disease #ClinicalTrial http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>Please RT: We're decoding the mystery of #disease @KeckMedUSC  &amp; are looking for study participants #ClinicalTrial http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>#disease e-patients: We're looking for your help. Researchers @KeckMedUSC are looking for #ClinicalTrial  volunteers http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>Join researcher Principal Investigator's Name @KeckMedUSC in fighting #disease. Share this #ClinicalTrial http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>You may be eligible to aid in this #ClinicalTrial on #disease @KeckMedUSC. We'd appreciate your help http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>If you've been diagnosed with #disease, you could help us fight it. Participate in this #ClinicalTrial @KeckMedUSC  http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>Ever wanted to participate in a #ClinicalTrial? Here's your chance to help advance #disease research http://bit.ly/1234567 @KeckMedUSC</t>
+  </si>
+  <si>
+    <t>You're more than your #disease. And you may be a unique way to fight it. Participate in #ClinicalTrial @KeckMedUSC http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We cannot  find better #disease treatments without you. If you're eligible, pls participate @KeckMedUSC http://bit.ly/1234567 </t>
+  </si>
+  <si>
+    <t>You can make a difference in others' lives. Please participate in our #ClinicalTrial on  #disease @KeckMedUSC http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>Join Principal Investigator's Name in fighting #disease by participating in this #ClinicalTrial @KeckMedUSC http://bit.ly/1234567</t>
+  </si>
+  <si>
+    <t>Diagnosed with #disease? Leading researcher PI's Name @KeckMedUSC is looking for #ClinicalTrial participants http://bit.ly/1234567</t>
   </si>
 </sst>
 </file>
@@ -709,7 +709,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -738,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -752,10 +752,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -769,7 +769,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -786,10 +786,10 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -803,10 +803,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -820,10 +820,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -837,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -857,7 +857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -871,7 +871,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -891,7 +891,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -905,7 +905,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -959,7 +959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -973,10 +973,10 @@
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -990,10 +990,10 @@
         <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1004,10 +1004,10 @@
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1021,13 +1021,13 @@
         <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1038,13 +1038,13 @@
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1055,13 +1055,13 @@
         <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1072,13 +1072,13 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1089,13 +1089,13 @@
         <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1109,10 +1109,10 @@
         <v>22</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1123,13 +1123,13 @@
         <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1157,10 +1157,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1191,10 +1191,10 @@
         <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1208,10 +1208,10 @@
         <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1225,13 +1225,13 @@
         <v>5</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1242,13 +1242,13 @@
         <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1256,16 +1256,16 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1273,16 +1273,16 @@
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1290,16 +1290,16 @@
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1307,16 +1307,16 @@
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1324,16 +1324,16 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1341,16 +1341,16 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1358,16 +1358,16 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1375,16 +1375,16 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1392,13 +1392,13 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1409,16 +1409,16 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1426,16 +1426,16 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1443,16 +1443,16 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1460,16 +1460,16 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1477,16 +1477,16 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1494,16 +1494,16 @@
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1511,16 +1511,16 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1528,16 +1528,16 @@
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1545,16 +1545,16 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1562,13 +1562,13 @@
         <v>4</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1579,13 +1579,13 @@
         <v>4</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E51" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1596,13 +1596,13 @@
         <v>4</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E52" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1613,13 +1613,13 @@
         <v>4</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1630,13 +1630,13 @@
         <v>4</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1647,13 +1647,13 @@
         <v>4</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E55" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1664,16 +1664,16 @@
         <v>4</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E56" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1681,16 +1681,16 @@
         <v>4</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1698,16 +1698,16 @@
         <v>4</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1715,16 +1715,16 @@
         <v>4</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1732,16 +1732,16 @@
         <v>4</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1749,13 +1749,13 @@
         <v>4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>